<commit_message>
Atualização do arquivo de pareceres
</commit_message>
<xml_diff>
--- a/04_contPareceres.xlsx
+++ b/04_contPareceres.xlsx
@@ -35702,13 +35702,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4EA3080-3420-4D0C-921B-F6B15833BA03}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52A3B13F-16A6-4E77-9208-6E5348B958E0}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A910A40-88A7-46CA-AF86-F60CC07FCDE7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F12D409-67D8-411A-A0D3-17CA8B8E3E9A}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5836467E-9D2E-4CD3-82CC-147294794DE4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C0EF103-CAE4-4253-A2D2-18A1090414BA}"/>
 </file>
</xml_diff>